<commit_message>
fixed row colors with conditional formatting
</commit_message>
<xml_diff>
--- a/uploads/Math.xlsx
+++ b/uploads/Math.xlsx
@@ -24,22 +24,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="b9ff9c"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="eb4034"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,15 +44,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="b9ff9c"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="eb4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="b9ff9c"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="eb4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -380,73 +397,93 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>12</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1">
         <v>3</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2.5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>1.9</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:C6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>=$C1=$A1+$B1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C6">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>=$C1=$A1+$B1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C6">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>=$C1=$A1+$B1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C6">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>=$C1&lt;&gt;$A1+$B1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct wrong values to column D
</commit_message>
<xml_diff>
--- a/uploads/Math.xlsx
+++ b/uploads/Math.xlsx
@@ -4,13 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2115" windowWidth="21600" windowHeight="11505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+  <si>
+    <t/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24,15 +32,20 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8C00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +53,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -54,14 +75,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="b9ff9c"/>
+          <bgColor rgb="FFB9FF9C"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="eb4034"/>
+          <bgColor rgb="FFEB4034"/>
         </patternFill>
       </fill>
     </dxf>
@@ -389,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>12</v>
       </c>
@@ -407,8 +428,11 @@
       <c r="C1">
         <v>15</v>
       </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -416,10 +440,13 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -429,8 +456,11 @@
       <c r="C3">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -440,8 +470,11 @@
       <c r="C4">
         <v>4.5</v>
       </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -451,8 +484,11 @@
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -461,17 +497,20 @@
       </c>
       <c r="C6">
         <v>1.9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C6">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>=$C1=$A1+$B1</formula>
+      <formula>$C1=$A1+$B1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C6">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>=$C1=$A1+$B1</formula>
+      <formula>$C1&lt;&gt;$A1+$B1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C6">

</xml_diff>

<commit_message>
excel validation bug fixes
</commit_message>
<xml_diff>
--- a/uploads/Math.xlsx
+++ b/uploads/Math.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t/>
+  </si>
+  <si>
+    <t>AS</t>
   </si>
 </sst>
 </file>
@@ -32,20 +35,15 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8C00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -53,25 +51,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -89,6 +79,139 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB9FF9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFEB4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor rgb="b9ff9c"/>
         </patternFill>
       </fill>
@@ -97,6 +220,13 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="eb4034"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFA500"/>
         </patternFill>
       </fill>
     </dxf>
@@ -410,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -440,10 +570,10 @@
         <v>10</v>
       </c>
       <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -484,7 +614,7 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>4</v>
       </c>
     </row>
@@ -498,29 +628,137 @@
       <c r="C6">
         <v>1.9</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C6">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$C1=$A1+$B1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C6">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$C1&lt;&gt;$A1+$B1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C6">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>=$C1=$A1+$B1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C6">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>=$C1&lt;&gt;$A1+$B1</formula>
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A:C">
+    <cfRule type="expression" dxfId="21" priority="21">
+      <formula>=AND($C1=$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A:C">
+    <cfRule type="expression" dxfId="22" priority="22">
+      <formula>=AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D:D">
+    <cfRule type="expression" dxfId="23" priority="23">
+      <formula>=AND($C1&lt;&gt;$A1+$B1, ISNUMBER($A1:$C1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>